<commit_message>
10,4 de 12,5 nota final
</commit_message>
<xml_diff>
--- a/Provas/MPT_01_SistemaBD/MPT_01_SistemaBD/FA-MPT-01-SEv1.xlsx
+++ b/Provas/MPT_01_SistemaBD/MPT_01_SistemaBD/FA-MPT-01-SEv1.xlsx
@@ -1,43 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\android\Documents\GitHub\WorldSkills\Provas\MPT_01_SistemaBD\MPT_01_SistemaBD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MulinhaGPlays\Documents\GitHub\WorldSkills\Provas\MPT_01_SistemaBD\MPT_01_SistemaBD\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A8E4B5-494A-429A-B7BD-7ACF9E127C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CIS_Subcriteria_Import" sheetId="4" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Peter Neate</author>
   </authors>
   <commentList>
-    <comment ref="D2" authorId="0" shapeId="0">
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -474,7 +462,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -652,7 +640,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -685,64 +673,65 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="12" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1108,11 +1097,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J67"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="B73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1163,7 +1152,7 @@
       <c r="D6" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="16">
         <v>10.75</v>
       </c>
     </row>
@@ -1174,7 +1163,7 @@
       <c r="D7" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="16">
         <v>0.5</v>
       </c>
     </row>
@@ -1185,7 +1174,7 @@
       <c r="D8" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="16">
         <v>1.25</v>
       </c>
     </row>
@@ -1196,23 +1185,23 @@
       <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:10" ht="41.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="26" t="s">
+      <c r="E11" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="27"/>
-      <c r="G11" s="24" t="s">
+      <c r="F11" s="26"/>
+      <c r="G11" s="23" t="s">
         <v>6</v>
       </c>
       <c r="H11" s="1" t="s">
@@ -1227,38 +1216,38 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="25"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
+      <c r="A12" s="24"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
       <c r="E12" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="25"/>
-      <c r="I12" s="16"/>
+      <c r="G12" s="24"/>
+      <c r="I12" s="14"/>
       <c r="J12" s="4"/>
     </row>
     <row r="13" spans="1:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="10">
         <v>1</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29" t="s">
+      <c r="E13" s="18"/>
+      <c r="F13" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="32">
+      <c r="G13" s="21">
         <v>0.2</v>
       </c>
       <c r="H13" s="4">
@@ -1266,22 +1255,22 @@
         <v>10.749999999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A14" s="10">
         <v>2</v>
       </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="28" t="s">
+      <c r="B14" s="22"/>
+      <c r="C14" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="29" t="s">
+      <c r="D14" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29" t="s">
+      <c r="E14" s="18"/>
+      <c r="F14" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="30">
+      <c r="G14" s="19">
         <v>0.2</v>
       </c>
     </row>
@@ -1289,18 +1278,18 @@
       <c r="A15" s="10">
         <v>3</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="28" t="s">
+      <c r="B15" s="22"/>
+      <c r="C15" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29" t="s">
+      <c r="E15" s="18"/>
+      <c r="F15" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="G15" s="30">
+      <c r="G15" s="19">
         <v>0.2</v>
       </c>
     </row>
@@ -1308,20 +1297,20 @@
       <c r="A16" s="10">
         <v>4</v>
       </c>
-      <c r="B16" s="23"/>
-      <c r="C16" s="28" t="s">
+      <c r="B16" s="22"/>
+      <c r="C16" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="29" t="s">
+      <c r="D16" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="29" t="s">
+      <c r="E16" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="F16" s="29" t="s">
+      <c r="F16" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="G16" s="30">
+      <c r="G16" s="19">
         <v>0.2</v>
       </c>
     </row>
@@ -1329,41 +1318,41 @@
       <c r="A17" s="10">
         <v>5</v>
       </c>
-      <c r="B17" s="23"/>
-      <c r="C17" s="28" t="s">
+      <c r="B17" s="22"/>
+      <c r="C17" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="29" t="s">
+      <c r="D17" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="29" t="s">
+      <c r="E17" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="F17" s="29" t="s">
+      <c r="F17" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G17" s="30">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="G17" s="19">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A18" s="10">
         <v>6</v>
       </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="28" t="s">
+      <c r="B18" s="22"/>
+      <c r="C18" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="29" t="s">
+      <c r="D18" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="29" t="s">
+      <c r="E18" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="F18" s="29" t="s">
+      <c r="F18" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="G18" s="30">
+      <c r="G18" s="19">
         <v>0.3</v>
       </c>
     </row>
@@ -1371,41 +1360,42 @@
       <c r="A19" s="10">
         <v>7</v>
       </c>
-      <c r="B19" s="23"/>
-      <c r="C19" s="28" t="s">
+      <c r="B19" s="22"/>
+      <c r="C19" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="29" t="s">
+      <c r="D19" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="29" t="s">
+      <c r="E19" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="F19" s="29" t="s">
+      <c r="F19" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="G19" s="30">
-        <v>0.2</v>
-      </c>
+      <c r="G19" s="19">
+        <v>0.2</v>
+      </c>
+      <c r="H19" s="30"/>
     </row>
     <row r="20" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A20" s="10">
         <v>8</v>
       </c>
-      <c r="B20" s="23"/>
-      <c r="C20" s="28" t="s">
+      <c r="B20" s="22"/>
+      <c r="C20" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="29" t="s">
+      <c r="D20" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="E20" s="29" t="s">
+      <c r="E20" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="F20" s="29" t="s">
+      <c r="F20" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="G20" s="30">
+      <c r="G20" s="19">
         <v>0.3</v>
       </c>
     </row>
@@ -1413,20 +1403,20 @@
       <c r="A21" s="10">
         <v>9</v>
       </c>
-      <c r="B21" s="23"/>
-      <c r="C21" s="19" t="s">
+      <c r="B21" s="22"/>
+      <c r="C21" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="20" t="s">
+      <c r="D21" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E21" s="20" t="s">
+      <c r="E21" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="20" t="s">
+      <c r="F21" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="G21" s="22">
+      <c r="G21" s="19">
         <v>0.3</v>
       </c>
     </row>
@@ -1434,20 +1424,20 @@
       <c r="A22" s="10">
         <v>10</v>
       </c>
-      <c r="B22" s="23"/>
-      <c r="C22" s="19" t="s">
+      <c r="B22" s="22"/>
+      <c r="C22" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="20" t="s">
+      <c r="D22" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="E22" s="20" t="s">
+      <c r="E22" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="F22" s="20" t="s">
+      <c r="F22" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="G22" s="22">
+      <c r="G22" s="19">
         <v>0.2</v>
       </c>
     </row>
@@ -1455,39 +1445,39 @@
       <c r="A23" s="10">
         <v>11</v>
       </c>
-      <c r="B23" s="23"/>
-      <c r="C23" s="19" t="s">
+      <c r="B23" s="22"/>
+      <c r="C23" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="20" t="s">
+      <c r="D23" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20" t="s">
+      <c r="E23" s="18"/>
+      <c r="F23" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="G23" s="22">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="G23" s="19">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A24" s="10">
         <v>12</v>
       </c>
-      <c r="B24" s="23"/>
-      <c r="C24" s="28" t="s">
+      <c r="B24" s="22"/>
+      <c r="C24" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="29" t="s">
+      <c r="D24" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="E24" s="29" t="s">
+      <c r="E24" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="F24" s="29" t="s">
+      <c r="F24" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="G24" s="30">
+      <c r="G24" s="19">
         <v>0.5</v>
       </c>
     </row>
@@ -1495,16 +1485,16 @@
       <c r="A25" s="10">
         <v>13</v>
       </c>
-      <c r="B25" s="23"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="29" t="s">
+      <c r="B25" s="22"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29" t="s">
+      <c r="E25" s="18"/>
+      <c r="F25" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="G25" s="30">
+      <c r="G25" s="19">
         <v>0.2</v>
       </c>
     </row>
@@ -1512,52 +1502,52 @@
       <c r="A26" s="10">
         <v>14</v>
       </c>
-      <c r="B26" s="23"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="29" t="s">
+      <c r="B26" s="22"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29" t="s">
+      <c r="E26" s="18"/>
+      <c r="F26" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="G26" s="30">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="G26" s="19">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="10">
         <v>15</v>
       </c>
-      <c r="B27" s="23"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="29" t="s">
+      <c r="B27" s="22"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="E27" s="29" t="s">
+      <c r="E27" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="F27" s="29" t="s">
+      <c r="F27" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="G27" s="30">
+      <c r="G27" s="19">
         <v>0.3</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A28" s="10">
         <v>16</v>
       </c>
-      <c r="B28" s="23"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="29" t="s">
+      <c r="B28" s="22"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29" t="s">
+      <c r="E28" s="18"/>
+      <c r="F28" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="G28" s="30">
+      <c r="G28" s="19">
         <v>0.15</v>
       </c>
     </row>
@@ -1565,34 +1555,34 @@
       <c r="A29" s="10">
         <v>17</v>
       </c>
-      <c r="B29" s="23"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="20" t="s">
+      <c r="B29" s="22"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20" t="s">
+      <c r="E29" s="18"/>
+      <c r="F29" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="G29" s="22">
+      <c r="G29" s="19">
         <v>0.15</v>
       </c>
-      <c r="H29" s="17"/>
+      <c r="H29" s="15"/>
     </row>
     <row r="30" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A30" s="10">
         <v>18</v>
       </c>
-      <c r="B30" s="23"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="20" t="s">
+      <c r="B30" s="22"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20" t="s">
+      <c r="E30" s="18"/>
+      <c r="F30" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="G30" s="22">
+      <c r="G30" s="19">
         <v>0.2</v>
       </c>
     </row>
@@ -1600,18 +1590,18 @@
       <c r="A31" s="10">
         <v>19</v>
       </c>
-      <c r="B31" s="23"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="20" t="s">
+      <c r="B31" s="22"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="E31" s="20" t="s">
+      <c r="E31" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="F31" s="20" t="s">
+      <c r="F31" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="G31" s="22">
+      <c r="G31" s="19">
         <v>0.5</v>
       </c>
     </row>
@@ -1619,14 +1609,14 @@
       <c r="A32" s="10">
         <v>20</v>
       </c>
-      <c r="B32" s="23"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="20" t="s">
+      <c r="B32" s="22"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="22">
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="19">
         <v>0.2</v>
       </c>
     </row>
@@ -1634,33 +1624,33 @@
       <c r="A33" s="10">
         <v>21</v>
       </c>
-      <c r="B33" s="23"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="20" t="s">
+      <c r="B33" s="22"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20" t="s">
+      <c r="E33" s="18"/>
+      <c r="F33" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="G33" s="22">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="G33" s="19">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" s="10">
         <v>22</v>
       </c>
-      <c r="B34" s="23"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="20" t="s">
+      <c r="B34" s="22"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20" t="s">
+      <c r="E34" s="18"/>
+      <c r="F34" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="G34" s="22">
+      <c r="G34" s="19">
         <v>0.2</v>
       </c>
     </row>
@@ -1668,16 +1658,16 @@
       <c r="A35" s="10">
         <v>23</v>
       </c>
-      <c r="B35" s="23"/>
-      <c r="C35" s="19"/>
-      <c r="D35" s="20" t="s">
+      <c r="B35" s="22"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20" t="s">
+      <c r="E35" s="11"/>
+      <c r="F35" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="G35" s="22">
+      <c r="G35" s="12">
         <v>0.1</v>
       </c>
     </row>
@@ -1685,18 +1675,18 @@
       <c r="A36" s="10">
         <v>24</v>
       </c>
-      <c r="B36" s="23"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="11" t="s">
+      <c r="B36" s="22"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="E36" s="11" t="s">
+      <c r="E36" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="F36" s="11" t="s">
+      <c r="F36" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="G36" s="13">
+      <c r="G36" s="19">
         <v>0.2</v>
       </c>
     </row>
@@ -1704,16 +1694,16 @@
       <c r="A37" s="10">
         <v>25</v>
       </c>
-      <c r="B37" s="23"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="20" t="s">
+      <c r="B37" s="22"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="E37" s="20"/>
-      <c r="F37" s="20" t="s">
+      <c r="E37" s="18"/>
+      <c r="F37" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="G37" s="22">
+      <c r="G37" s="19">
         <v>0.2</v>
       </c>
     </row>
@@ -1721,16 +1711,16 @@
       <c r="A38" s="10">
         <v>26</v>
       </c>
-      <c r="B38" s="23"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="20" t="s">
+      <c r="B38" s="22"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20" t="s">
+      <c r="E38" s="18"/>
+      <c r="F38" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="G38" s="22">
+      <c r="G38" s="19">
         <v>0.2</v>
       </c>
     </row>
@@ -1738,31 +1728,31 @@
       <c r="A39" s="10">
         <v>27</v>
       </c>
-      <c r="B39" s="23"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="20" t="s">
+      <c r="B39" s="22"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="E39" s="20"/>
-      <c r="F39" s="20" t="s">
+      <c r="E39" s="18"/>
+      <c r="F39" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="G39" s="22">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="G39" s="19">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="10">
         <v>28</v>
       </c>
-      <c r="B40" s="23"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="20" t="s">
+      <c r="B40" s="22"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="22">
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="19">
         <v>0.1</v>
       </c>
     </row>
@@ -1770,16 +1760,16 @@
       <c r="A41" s="10">
         <v>29</v>
       </c>
-      <c r="B41" s="23"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="20" t="s">
+      <c r="B41" s="22"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20" t="s">
+      <c r="E41" s="18"/>
+      <c r="F41" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="G41" s="22">
+      <c r="G41" s="19">
         <v>0.2</v>
       </c>
     </row>
@@ -1787,33 +1777,33 @@
       <c r="A42" s="10">
         <v>30</v>
       </c>
-      <c r="B42" s="23"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="20" t="s">
+      <c r="B42" s="22"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="E42" s="20" t="s">
+      <c r="E42" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="F42" s="20" t="s">
+      <c r="F42" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="G42" s="22">
+      <c r="G42" s="19">
         <v>0.4</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="10">
         <v>31</v>
       </c>
-      <c r="B43" s="23"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="11" t="s">
+      <c r="B43" s="22"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E43" s="11"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="13">
+      <c r="E43" s="18"/>
+      <c r="F43" s="18"/>
+      <c r="G43" s="19">
         <v>0.2</v>
       </c>
     </row>
@@ -1821,43 +1811,43 @@
       <c r="A44" s="10">
         <v>32</v>
       </c>
-      <c r="B44" s="23"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="11" t="s">
+      <c r="B44" s="22"/>
+      <c r="C44" s="17"/>
+      <c r="D44" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="E44" s="11" t="s">
+      <c r="E44" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="F44" s="11"/>
-      <c r="G44" s="13">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="F44" s="18"/>
+      <c r="G44" s="19">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A45" s="10">
         <v>33</v>
       </c>
-      <c r="B45" s="23"/>
-      <c r="C45" s="10"/>
-      <c r="D45" s="11" t="s">
+      <c r="B45" s="22"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="E45" s="11" t="s">
+      <c r="E45" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="F45" s="11" t="s">
+      <c r="F45" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="G45" s="13">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="G45" s="29">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A46" s="10">
         <v>34</v>
       </c>
-      <c r="B46" s="23"/>
+      <c r="B46" s="22"/>
       <c r="C46" s="10"/>
       <c r="D46" s="11" t="s">
         <v>100</v>
@@ -1866,7 +1856,7 @@
       <c r="F46" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="G46" s="13">
+      <c r="G46" s="12">
         <v>0.2</v>
       </c>
     </row>
@@ -1874,7 +1864,7 @@
       <c r="A47" s="10">
         <v>35</v>
       </c>
-      <c r="B47" s="23"/>
+      <c r="B47" s="22"/>
       <c r="C47" s="10"/>
       <c r="D47" s="11" t="s">
         <v>102</v>
@@ -1883,7 +1873,7 @@
         <v>60</v>
       </c>
       <c r="F47" s="11"/>
-      <c r="G47" s="13">
+      <c r="G47" s="12">
         <v>0.3</v>
       </c>
     </row>
@@ -1891,14 +1881,14 @@
       <c r="A48" s="10">
         <v>36</v>
       </c>
-      <c r="B48" s="23"/>
+      <c r="B48" s="22"/>
       <c r="C48" s="10"/>
       <c r="D48" s="11" t="s">
         <v>103</v>
       </c>
       <c r="E48" s="11"/>
       <c r="F48" s="11"/>
-      <c r="G48" s="13">
+      <c r="G48" s="12">
         <v>0.2</v>
       </c>
     </row>
@@ -1906,14 +1896,14 @@
       <c r="A49" s="10">
         <v>37</v>
       </c>
-      <c r="B49" s="23"/>
-      <c r="C49" s="10"/>
-      <c r="D49" s="11" t="s">
+      <c r="B49" s="22"/>
+      <c r="C49" s="17"/>
+      <c r="D49" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="E49" s="11"/>
-      <c r="F49" s="11"/>
-      <c r="G49" s="13">
+      <c r="E49" s="18"/>
+      <c r="F49" s="18"/>
+      <c r="G49" s="19">
         <v>0.2</v>
       </c>
     </row>
@@ -1921,14 +1911,14 @@
       <c r="A50" s="10">
         <v>38</v>
       </c>
-      <c r="B50" s="23"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="11" t="s">
+      <c r="B50" s="22"/>
+      <c r="C50" s="27"/>
+      <c r="D50" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="E50" s="11"/>
-      <c r="F50" s="11"/>
-      <c r="G50" s="13">
+      <c r="E50" s="28"/>
+      <c r="F50" s="28"/>
+      <c r="G50" s="29">
         <v>0.2</v>
       </c>
     </row>
@@ -1936,14 +1926,14 @@
       <c r="A51" s="10">
         <v>39</v>
       </c>
-      <c r="B51" s="23"/>
+      <c r="B51" s="22"/>
       <c r="C51" s="10"/>
       <c r="D51" s="11" t="s">
         <v>109</v>
       </c>
       <c r="E51" s="11"/>
       <c r="F51" s="11"/>
-      <c r="G51" s="13">
+      <c r="G51" s="12">
         <v>0.2</v>
       </c>
     </row>
@@ -1951,14 +1941,14 @@
       <c r="A52" s="10">
         <v>40</v>
       </c>
-      <c r="B52" s="23"/>
+      <c r="B52" s="22"/>
       <c r="C52" s="10"/>
       <c r="D52" s="11" t="s">
         <v>106</v>
       </c>
       <c r="E52" s="11"/>
       <c r="F52" s="11"/>
-      <c r="G52" s="13">
+      <c r="G52" s="12">
         <v>0.2</v>
       </c>
     </row>
@@ -1966,14 +1956,14 @@
       <c r="A53" s="10">
         <v>41</v>
       </c>
-      <c r="B53" s="23"/>
+      <c r="B53" s="22"/>
       <c r="C53" s="10"/>
       <c r="D53" s="11" t="s">
         <v>107</v>
       </c>
       <c r="E53" s="11"/>
       <c r="F53" s="11"/>
-      <c r="G53" s="13">
+      <c r="G53" s="12">
         <v>0.2</v>
       </c>
     </row>
@@ -1981,14 +1971,14 @@
       <c r="A54" s="10">
         <v>42</v>
       </c>
-      <c r="B54" s="23"/>
-      <c r="C54" s="10"/>
-      <c r="D54" s="11" t="s">
+      <c r="B54" s="22"/>
+      <c r="C54" s="17"/>
+      <c r="D54" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="E54" s="11"/>
-      <c r="F54" s="11"/>
-      <c r="G54" s="13">
+      <c r="E54" s="18"/>
+      <c r="F54" s="18"/>
+      <c r="G54" s="19">
         <v>0.15</v>
       </c>
     </row>
@@ -1996,16 +1986,16 @@
       <c r="A55" s="10">
         <v>43</v>
       </c>
-      <c r="B55" s="23"/>
-      <c r="C55" s="28"/>
-      <c r="D55" s="29" t="s">
+      <c r="B55" s="22"/>
+      <c r="C55" s="17"/>
+      <c r="D55" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="E55" s="29"/>
-      <c r="F55" s="29" t="s">
+      <c r="E55" s="18"/>
+      <c r="F55" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="G55" s="30">
+      <c r="G55" s="19">
         <v>0.3</v>
       </c>
     </row>
@@ -2013,16 +2003,16 @@
       <c r="A56" s="10">
         <v>44</v>
       </c>
-      <c r="B56" s="23"/>
-      <c r="C56" s="28"/>
-      <c r="D56" s="29" t="s">
+      <c r="B56" s="22"/>
+      <c r="C56" s="17"/>
+      <c r="D56" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="E56" s="29"/>
-      <c r="F56" s="29" t="s">
+      <c r="E56" s="18"/>
+      <c r="F56" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="G56" s="30">
+      <c r="G56" s="19">
         <v>0.3</v>
       </c>
     </row>
@@ -2030,16 +2020,16 @@
       <c r="A57" s="10">
         <v>45</v>
       </c>
-      <c r="B57" s="23"/>
-      <c r="C57" s="28"/>
-      <c r="D57" s="29" t="s">
+      <c r="B57" s="22"/>
+      <c r="C57" s="17"/>
+      <c r="D57" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="E57" s="29"/>
-      <c r="F57" s="29" t="s">
+      <c r="E57" s="18"/>
+      <c r="F57" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="G57" s="30">
+      <c r="G57" s="19">
         <v>0.2</v>
       </c>
     </row>
@@ -2047,14 +2037,14 @@
       <c r="A58" s="10">
         <v>46</v>
       </c>
-      <c r="B58" s="23"/>
-      <c r="C58" s="28"/>
-      <c r="D58" s="29" t="s">
+      <c r="B58" s="22"/>
+      <c r="C58" s="17"/>
+      <c r="D58" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="E58" s="29"/>
-      <c r="F58" s="29"/>
-      <c r="G58" s="30">
+      <c r="E58" s="18"/>
+      <c r="F58" s="18"/>
+      <c r="G58" s="19">
         <v>0.2</v>
       </c>
     </row>
@@ -2062,16 +2052,16 @@
       <c r="A59" s="10">
         <v>47</v>
       </c>
-      <c r="B59" s="23"/>
-      <c r="C59" s="28"/>
-      <c r="D59" s="29" t="s">
+      <c r="B59" s="22"/>
+      <c r="C59" s="17"/>
+      <c r="D59" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="E59" s="29"/>
-      <c r="F59" s="29" t="s">
+      <c r="E59" s="18"/>
+      <c r="F59" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="G59" s="30">
+      <c r="G59" s="19">
         <v>0.2</v>
       </c>
     </row>
@@ -2079,16 +2069,16 @@
       <c r="A60" s="10">
         <v>48</v>
       </c>
-      <c r="B60" s="23"/>
-      <c r="C60" s="28"/>
-      <c r="D60" s="29" t="s">
+      <c r="B60" s="22"/>
+      <c r="C60" s="17"/>
+      <c r="D60" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="E60" s="29"/>
-      <c r="F60" s="29" t="s">
+      <c r="E60" s="18"/>
+      <c r="F60" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="G60" s="30">
+      <c r="G60" s="19">
         <v>0.2</v>
       </c>
     </row>
@@ -2096,22 +2086,22 @@
       <c r="A61" s="10">
         <v>49</v>
       </c>
-      <c r="B61" s="23" t="s">
+      <c r="B61" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C61" s="19" t="s">
+      <c r="C61" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D61" s="20" t="s">
+      <c r="D61" s="18" t="s">
         <v>28</v>
       </c>
       <c r="E61" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="F61" s="20" t="s">
+      <c r="F61" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="G61" s="22">
+      <c r="G61" s="19">
         <v>0.4</v>
       </c>
       <c r="I61" s="4"/>
@@ -2120,20 +2110,20 @@
       <c r="A62" s="10">
         <v>50</v>
       </c>
-      <c r="B62" s="23"/>
-      <c r="C62" s="19" t="s">
+      <c r="B62" s="22"/>
+      <c r="C62" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D62" s="20" t="s">
+      <c r="D62" s="18" t="s">
         <v>29</v>
       </c>
       <c r="E62" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="F62" s="20" t="s">
+      <c r="F62" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="G62" s="22">
+      <c r="G62" s="19">
         <v>0.25</v>
       </c>
     </row>
@@ -2141,20 +2131,20 @@
       <c r="A63" s="10">
         <v>51</v>
       </c>
-      <c r="B63" s="23"/>
-      <c r="C63" s="10" t="s">
+      <c r="B63" s="22"/>
+      <c r="C63" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D63" s="11" t="s">
+      <c r="D63" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E63" s="12" t="s">
+      <c r="E63" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="F63" s="11" t="s">
+      <c r="F63" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="G63" s="13">
+      <c r="G63" s="19">
         <v>0.3</v>
       </c>
     </row>
@@ -2162,20 +2152,20 @@
       <c r="A64" s="10">
         <v>52</v>
       </c>
-      <c r="B64" s="23"/>
-      <c r="C64" s="10" t="s">
+      <c r="B64" s="22"/>
+      <c r="C64" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D64" s="11" t="s">
+      <c r="D64" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E64" s="12" t="s">
+      <c r="E64" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="F64" s="11" t="s">
+      <c r="F64" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G64" s="13">
+      <c r="G64" s="19">
         <v>0.3</v>
       </c>
     </row>
@@ -2183,20 +2173,20 @@
       <c r="A65" s="10">
         <v>53</v>
       </c>
-      <c r="B65" s="23" t="s">
+      <c r="B65" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C65" s="10" t="s">
+      <c r="C65" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D65" s="11" t="s">
+      <c r="D65" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="E65" s="14"/>
-      <c r="F65" s="11" t="s">
+      <c r="E65" s="31"/>
+      <c r="F65" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G65" s="13">
+      <c r="G65" s="19">
         <v>0.1</v>
       </c>
     </row>
@@ -2204,16 +2194,16 @@
       <c r="A66" s="10">
         <v>54</v>
       </c>
-      <c r="B66" s="23"/>
-      <c r="C66" s="10" t="s">
+      <c r="B66" s="22"/>
+      <c r="C66" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D66" s="11" t="s">
+      <c r="D66" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="E66" s="14"/>
-      <c r="F66" s="15"/>
-      <c r="G66" s="13">
+      <c r="E66" s="32"/>
+      <c r="F66" s="33"/>
+      <c r="G66" s="29">
         <v>0.1</v>
       </c>
     </row>
@@ -2221,19 +2211,25 @@
       <c r="A67" s="10">
         <v>55</v>
       </c>
-      <c r="B67" s="23"/>
+      <c r="B67" s="22"/>
       <c r="C67" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D67" s="14" t="s">
+      <c r="D67" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E67" s="14"/>
+      <c r="E67" s="13"/>
       <c r="F67" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="G67" s="13">
+      <c r="G67" s="12">
         <v>0.3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G68">
+        <f>SUM(G13:G67)</f>
+        <v>12.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
o reinicio de tudo
</commit_message>
<xml_diff>
--- a/Provas/MPT_01_SistemaBD/MPT_01_SistemaBD/FA-MPT-01-SEv1.xlsx
+++ b/Provas/MPT_01_SistemaBD/MPT_01_SistemaBD/FA-MPT-01-SEv1.xlsx
@@ -1,31 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MulinhaGPlays\Documents\GitHub\WorldSkills\Provas\MPT_01_SistemaBD\MPT_01_SistemaBD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\android\Documents\GitHub\WorldSkills\Provas\MPT_01_SistemaBD\MPT_01_SistemaBD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A8E4B5-494A-429A-B7BD-7ACF9E127C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310"/>
   </bookViews>
   <sheets>
     <sheet name="CIS_Subcriteria_Import" sheetId="4" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Peter Neate</author>
   </authors>
   <commentList>
-    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="D2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -462,7 +461,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -558,7 +557,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
+        <fgColor rgb="FF00FF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -640,7 +639,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -670,34 +669,25 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="12" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -714,24 +704,15 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -739,6 +720,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF00FF00"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1097,11 +1083,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" topLeftCell="C10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1152,7 +1138,7 @@
       <c r="D6" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="16">
+      <c r="E6" s="13">
         <v>10.75</v>
       </c>
     </row>
@@ -1163,7 +1149,7 @@
       <c r="D7" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="13">
         <v>0.5</v>
       </c>
     </row>
@@ -1174,7 +1160,7 @@
       <c r="D8" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E8" s="13">
         <v>1.25</v>
       </c>
     </row>
@@ -1185,23 +1171,23 @@
       <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:10" ht="41.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="E11" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="26"/>
-      <c r="G11" s="23" t="s">
+      <c r="F11" s="23"/>
+      <c r="G11" s="20" t="s">
         <v>6</v>
       </c>
       <c r="H11" s="1" t="s">
@@ -1216,38 +1202,38 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="24"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
+      <c r="A12" s="21"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
       <c r="E12" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="24"/>
-      <c r="I12" s="14"/>
+      <c r="G12" s="21"/>
+      <c r="I12" s="11"/>
       <c r="J12" s="4"/>
     </row>
     <row r="13" spans="1:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="10">
         <v>1</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18" t="s">
+      <c r="E13" s="15"/>
+      <c r="F13" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="21">
+      <c r="G13" s="27">
         <v>0.2</v>
       </c>
       <c r="H13" s="4">
@@ -1259,18 +1245,18 @@
       <c r="A14" s="10">
         <v>2</v>
       </c>
-      <c r="B14" s="22"/>
-      <c r="C14" s="17" t="s">
+      <c r="B14" s="19"/>
+      <c r="C14" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="D14" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18" t="s">
+      <c r="E14" s="15"/>
+      <c r="F14" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="19">
+      <c r="G14" s="16">
         <v>0.2</v>
       </c>
     </row>
@@ -1278,18 +1264,18 @@
       <c r="A15" s="10">
         <v>3</v>
       </c>
-      <c r="B15" s="22"/>
-      <c r="C15" s="17" t="s">
+      <c r="B15" s="19"/>
+      <c r="C15" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18" t="s">
+      <c r="E15" s="15"/>
+      <c r="F15" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="G15" s="19">
+      <c r="G15" s="16">
         <v>0.2</v>
       </c>
     </row>
@@ -1297,20 +1283,20 @@
       <c r="A16" s="10">
         <v>4</v>
       </c>
-      <c r="B16" s="22"/>
-      <c r="C16" s="17" t="s">
+      <c r="B16" s="19"/>
+      <c r="C16" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="18" t="s">
+      <c r="E16" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="F16" s="18" t="s">
+      <c r="F16" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="G16" s="19">
+      <c r="G16" s="16">
         <v>0.2</v>
       </c>
     </row>
@@ -1318,20 +1304,20 @@
       <c r="A17" s="10">
         <v>5</v>
       </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="17" t="s">
+      <c r="B17" s="19"/>
+      <c r="C17" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="18" t="s">
+      <c r="E17" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="F17" s="18" t="s">
+      <c r="F17" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="G17" s="19">
+      <c r="G17" s="16">
         <v>0.2</v>
       </c>
     </row>
@@ -1339,20 +1325,20 @@
       <c r="A18" s="10">
         <v>6</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="17" t="s">
+      <c r="B18" s="19"/>
+      <c r="C18" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="18" t="s">
+      <c r="D18" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="18" t="s">
+      <c r="E18" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="F18" s="18" t="s">
+      <c r="F18" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="G18" s="19">
+      <c r="G18" s="16">
         <v>0.3</v>
       </c>
     </row>
@@ -1360,42 +1346,42 @@
       <c r="A19" s="10">
         <v>7</v>
       </c>
-      <c r="B19" s="22"/>
-      <c r="C19" s="17" t="s">
+      <c r="B19" s="19"/>
+      <c r="C19" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E19" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="F19" s="18" t="s">
+      <c r="F19" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="G19" s="19">
-        <v>0.2</v>
-      </c>
-      <c r="H19" s="30"/>
+      <c r="G19" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="H19" s="26"/>
     </row>
     <row r="20" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A20" s="10">
         <v>8</v>
       </c>
-      <c r="B20" s="22"/>
-      <c r="C20" s="17" t="s">
+      <c r="B20" s="19"/>
+      <c r="C20" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="E20" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="F20" s="18" t="s">
+      <c r="F20" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="G20" s="19">
+      <c r="G20" s="16">
         <v>0.3</v>
       </c>
     </row>
@@ -1403,20 +1389,20 @@
       <c r="A21" s="10">
         <v>9</v>
       </c>
-      <c r="B21" s="22"/>
-      <c r="C21" s="17" t="s">
+      <c r="B21" s="19"/>
+      <c r="C21" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="18" t="s">
+      <c r="D21" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="E21" s="18" t="s">
+      <c r="E21" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="18" t="s">
+      <c r="F21" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="G21" s="19">
+      <c r="G21" s="16">
         <v>0.3</v>
       </c>
     </row>
@@ -1424,20 +1410,20 @@
       <c r="A22" s="10">
         <v>10</v>
       </c>
-      <c r="B22" s="22"/>
-      <c r="C22" s="17" t="s">
+      <c r="B22" s="19"/>
+      <c r="C22" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="18" t="s">
+      <c r="D22" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="E22" s="18" t="s">
+      <c r="E22" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="F22" s="18" t="s">
+      <c r="F22" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="G22" s="19">
+      <c r="G22" s="16">
         <v>0.2</v>
       </c>
     </row>
@@ -1445,18 +1431,18 @@
       <c r="A23" s="10">
         <v>11</v>
       </c>
-      <c r="B23" s="22"/>
-      <c r="C23" s="17" t="s">
+      <c r="B23" s="19"/>
+      <c r="C23" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="18" t="s">
+      <c r="D23" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18" t="s">
+      <c r="E23" s="15"/>
+      <c r="F23" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="G23" s="19">
+      <c r="G23" s="16">
         <v>0.2</v>
       </c>
     </row>
@@ -1464,20 +1450,20 @@
       <c r="A24" s="10">
         <v>12</v>
       </c>
-      <c r="B24" s="22"/>
-      <c r="C24" s="17" t="s">
+      <c r="B24" s="19"/>
+      <c r="C24" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="18" t="s">
+      <c r="D24" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="E24" s="18" t="s">
+      <c r="E24" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="F24" s="18" t="s">
+      <c r="F24" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="G24" s="19">
+      <c r="G24" s="16">
         <v>0.5</v>
       </c>
     </row>
@@ -1485,16 +1471,16 @@
       <c r="A25" s="10">
         <v>13</v>
       </c>
-      <c r="B25" s="22"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="18" t="s">
+      <c r="B25" s="19"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18" t="s">
+      <c r="E25" s="15"/>
+      <c r="F25" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="G25" s="19">
+      <c r="G25" s="16">
         <v>0.2</v>
       </c>
     </row>
@@ -1502,16 +1488,16 @@
       <c r="A26" s="10">
         <v>14</v>
       </c>
-      <c r="B26" s="22"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="18" t="s">
+      <c r="B26" s="19"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18" t="s">
+      <c r="E26" s="15"/>
+      <c r="F26" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="G26" s="19">
+      <c r="G26" s="16">
         <v>0.2</v>
       </c>
     </row>
@@ -1519,18 +1505,18 @@
       <c r="A27" s="10">
         <v>15</v>
       </c>
-      <c r="B27" s="22"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="18" t="s">
+      <c r="B27" s="19"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="E27" s="18" t="s">
+      <c r="E27" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="F27" s="18" t="s">
+      <c r="F27" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="G27" s="19">
+      <c r="G27" s="16">
         <v>0.3</v>
       </c>
     </row>
@@ -1538,16 +1524,16 @@
       <c r="A28" s="10">
         <v>16</v>
       </c>
-      <c r="B28" s="22"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="18" t="s">
+      <c r="B28" s="19"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18" t="s">
+      <c r="E28" s="15"/>
+      <c r="F28" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="G28" s="19">
+      <c r="G28" s="16">
         <v>0.15</v>
       </c>
     </row>
@@ -1555,34 +1541,34 @@
       <c r="A29" s="10">
         <v>17</v>
       </c>
-      <c r="B29" s="22"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="18" t="s">
+      <c r="B29" s="19"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18" t="s">
+      <c r="E29" s="15"/>
+      <c r="F29" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="G29" s="19">
+      <c r="G29" s="16">
         <v>0.15</v>
       </c>
-      <c r="H29" s="15"/>
+      <c r="H29" s="12"/>
     </row>
     <row r="30" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A30" s="10">
         <v>18</v>
       </c>
-      <c r="B30" s="22"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="18" t="s">
+      <c r="B30" s="19"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18" t="s">
+      <c r="E30" s="15"/>
+      <c r="F30" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="G30" s="19">
+      <c r="G30" s="16">
         <v>0.2</v>
       </c>
     </row>
@@ -1590,18 +1576,18 @@
       <c r="A31" s="10">
         <v>19</v>
       </c>
-      <c r="B31" s="22"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="18" t="s">
+      <c r="B31" s="19"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="E31" s="18" t="s">
+      <c r="E31" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="F31" s="18" t="s">
+      <c r="F31" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="G31" s="19">
+      <c r="G31" s="16">
         <v>0.5</v>
       </c>
     </row>
@@ -1609,14 +1595,14 @@
       <c r="A32" s="10">
         <v>20</v>
       </c>
-      <c r="B32" s="22"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="18" t="s">
+      <c r="B32" s="19"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="19">
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="16">
         <v>0.2</v>
       </c>
     </row>
@@ -1624,16 +1610,16 @@
       <c r="A33" s="10">
         <v>21</v>
       </c>
-      <c r="B33" s="22"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="18" t="s">
+      <c r="B33" s="19"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18" t="s">
+      <c r="E33" s="15"/>
+      <c r="F33" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="G33" s="19">
+      <c r="G33" s="16">
         <v>0.2</v>
       </c>
     </row>
@@ -1641,16 +1627,16 @@
       <c r="A34" s="10">
         <v>22</v>
       </c>
-      <c r="B34" s="22"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="18" t="s">
+      <c r="B34" s="19"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18" t="s">
+      <c r="E34" s="15"/>
+      <c r="F34" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="G34" s="19">
+      <c r="G34" s="16">
         <v>0.2</v>
       </c>
     </row>
@@ -1658,16 +1644,16 @@
       <c r="A35" s="10">
         <v>23</v>
       </c>
-      <c r="B35" s="22"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="11" t="s">
+      <c r="B35" s="19"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11" t="s">
+      <c r="E35" s="15"/>
+      <c r="F35" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="G35" s="12">
+      <c r="G35" s="16">
         <v>0.1</v>
       </c>
     </row>
@@ -1675,18 +1661,18 @@
       <c r="A36" s="10">
         <v>24</v>
       </c>
-      <c r="B36" s="22"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="18" t="s">
+      <c r="B36" s="19"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="E36" s="18" t="s">
+      <c r="E36" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="F36" s="18" t="s">
+      <c r="F36" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="G36" s="19">
+      <c r="G36" s="16">
         <v>0.2</v>
       </c>
     </row>
@@ -1694,16 +1680,16 @@
       <c r="A37" s="10">
         <v>25</v>
       </c>
-      <c r="B37" s="22"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="18" t="s">
+      <c r="B37" s="19"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18" t="s">
+      <c r="E37" s="15"/>
+      <c r="F37" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="G37" s="19">
+      <c r="G37" s="16">
         <v>0.2</v>
       </c>
     </row>
@@ -1711,16 +1697,16 @@
       <c r="A38" s="10">
         <v>26</v>
       </c>
-      <c r="B38" s="22"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="18" t="s">
+      <c r="B38" s="19"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18" t="s">
+      <c r="E38" s="15"/>
+      <c r="F38" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="G38" s="19">
+      <c r="G38" s="16">
         <v>0.2</v>
       </c>
     </row>
@@ -1728,16 +1714,16 @@
       <c r="A39" s="10">
         <v>27</v>
       </c>
-      <c r="B39" s="22"/>
-      <c r="C39" s="17"/>
-      <c r="D39" s="18" t="s">
+      <c r="B39" s="19"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18" t="s">
+      <c r="E39" s="15"/>
+      <c r="F39" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="G39" s="19">
+      <c r="G39" s="16">
         <v>0.2</v>
       </c>
     </row>
@@ -1745,14 +1731,14 @@
       <c r="A40" s="10">
         <v>28</v>
       </c>
-      <c r="B40" s="22"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="18" t="s">
+      <c r="B40" s="19"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="19">
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="16">
         <v>0.1</v>
       </c>
     </row>
@@ -1760,16 +1746,16 @@
       <c r="A41" s="10">
         <v>29</v>
       </c>
-      <c r="B41" s="22"/>
-      <c r="C41" s="17"/>
-      <c r="D41" s="18" t="s">
+      <c r="B41" s="19"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18" t="s">
+      <c r="E41" s="15"/>
+      <c r="F41" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="G41" s="19">
+      <c r="G41" s="16">
         <v>0.2</v>
       </c>
     </row>
@@ -1777,18 +1763,18 @@
       <c r="A42" s="10">
         <v>30</v>
       </c>
-      <c r="B42" s="22"/>
-      <c r="C42" s="17"/>
-      <c r="D42" s="18" t="s">
+      <c r="B42" s="19"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="E42" s="18" t="s">
+      <c r="E42" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="F42" s="18" t="s">
+      <c r="F42" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="G42" s="19">
+      <c r="G42" s="16">
         <v>0.4</v>
       </c>
     </row>
@@ -1796,14 +1782,14 @@
       <c r="A43" s="10">
         <v>31</v>
       </c>
-      <c r="B43" s="22"/>
-      <c r="C43" s="17"/>
-      <c r="D43" s="18" t="s">
+      <c r="B43" s="19"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="19">
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="16">
         <v>0.2</v>
       </c>
     </row>
@@ -1811,16 +1797,16 @@
       <c r="A44" s="10">
         <v>32</v>
       </c>
-      <c r="B44" s="22"/>
-      <c r="C44" s="17"/>
-      <c r="D44" s="18" t="s">
+      <c r="B44" s="19"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="E44" s="18" t="s">
+      <c r="E44" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="F44" s="18"/>
-      <c r="G44" s="19">
+      <c r="F44" s="15"/>
+      <c r="G44" s="16">
         <v>0.2</v>
       </c>
     </row>
@@ -1828,18 +1814,18 @@
       <c r="A45" s="10">
         <v>33</v>
       </c>
-      <c r="B45" s="22"/>
-      <c r="C45" s="27"/>
-      <c r="D45" s="28" t="s">
+      <c r="B45" s="19"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="E45" s="28" t="s">
+      <c r="E45" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="F45" s="28" t="s">
+      <c r="F45" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="G45" s="29">
+      <c r="G45" s="16">
         <v>0.2</v>
       </c>
     </row>
@@ -1847,16 +1833,16 @@
       <c r="A46" s="10">
         <v>34</v>
       </c>
-      <c r="B46" s="22"/>
-      <c r="C46" s="10"/>
-      <c r="D46" s="11" t="s">
+      <c r="B46" s="19"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="E46" s="11"/>
-      <c r="F46" s="11" t="s">
+      <c r="E46" s="15"/>
+      <c r="F46" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="G46" s="12">
+      <c r="G46" s="16">
         <v>0.2</v>
       </c>
     </row>
@@ -1864,16 +1850,16 @@
       <c r="A47" s="10">
         <v>35</v>
       </c>
-      <c r="B47" s="22"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="11" t="s">
+      <c r="B47" s="19"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="E47" s="11" t="s">
+      <c r="E47" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="F47" s="11"/>
-      <c r="G47" s="12">
+      <c r="F47" s="15"/>
+      <c r="G47" s="16">
         <v>0.3</v>
       </c>
     </row>
@@ -1881,14 +1867,14 @@
       <c r="A48" s="10">
         <v>36</v>
       </c>
-      <c r="B48" s="22"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="11" t="s">
+      <c r="B48" s="19"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
-      <c r="G48" s="12">
+      <c r="E48" s="15"/>
+      <c r="F48" s="15"/>
+      <c r="G48" s="16">
         <v>0.2</v>
       </c>
     </row>
@@ -1896,14 +1882,14 @@
       <c r="A49" s="10">
         <v>37</v>
       </c>
-      <c r="B49" s="22"/>
-      <c r="C49" s="17"/>
-      <c r="D49" s="18" t="s">
+      <c r="B49" s="19"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="E49" s="18"/>
-      <c r="F49" s="18"/>
-      <c r="G49" s="19">
+      <c r="E49" s="15"/>
+      <c r="F49" s="15"/>
+      <c r="G49" s="16">
         <v>0.2</v>
       </c>
     </row>
@@ -1911,14 +1897,14 @@
       <c r="A50" s="10">
         <v>38</v>
       </c>
-      <c r="B50" s="22"/>
-      <c r="C50" s="27"/>
-      <c r="D50" s="28" t="s">
+      <c r="B50" s="19"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="E50" s="28"/>
-      <c r="F50" s="28"/>
-      <c r="G50" s="29">
+      <c r="E50" s="15"/>
+      <c r="F50" s="15"/>
+      <c r="G50" s="16">
         <v>0.2</v>
       </c>
     </row>
@@ -1926,14 +1912,14 @@
       <c r="A51" s="10">
         <v>39</v>
       </c>
-      <c r="B51" s="22"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="11" t="s">
+      <c r="B51" s="19"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="12">
+      <c r="E51" s="15"/>
+      <c r="F51" s="15"/>
+      <c r="G51" s="16">
         <v>0.2</v>
       </c>
     </row>
@@ -1941,14 +1927,14 @@
       <c r="A52" s="10">
         <v>40</v>
       </c>
-      <c r="B52" s="22"/>
-      <c r="C52" s="10"/>
-      <c r="D52" s="11" t="s">
+      <c r="B52" s="19"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="E52" s="11"/>
-      <c r="F52" s="11"/>
-      <c r="G52" s="12">
+      <c r="E52" s="15"/>
+      <c r="F52" s="15"/>
+      <c r="G52" s="16">
         <v>0.2</v>
       </c>
     </row>
@@ -1956,14 +1942,14 @@
       <c r="A53" s="10">
         <v>41</v>
       </c>
-      <c r="B53" s="22"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="11" t="s">
+      <c r="B53" s="19"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="E53" s="11"/>
-      <c r="F53" s="11"/>
-      <c r="G53" s="12">
+      <c r="E53" s="15"/>
+      <c r="F53" s="15"/>
+      <c r="G53" s="16">
         <v>0.2</v>
       </c>
     </row>
@@ -1971,14 +1957,14 @@
       <c r="A54" s="10">
         <v>42</v>
       </c>
-      <c r="B54" s="22"/>
-      <c r="C54" s="17"/>
-      <c r="D54" s="18" t="s">
+      <c r="B54" s="19"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="E54" s="18"/>
-      <c r="F54" s="18"/>
-      <c r="G54" s="19">
+      <c r="E54" s="15"/>
+      <c r="F54" s="15"/>
+      <c r="G54" s="16">
         <v>0.15</v>
       </c>
     </row>
@@ -1986,16 +1972,16 @@
       <c r="A55" s="10">
         <v>43</v>
       </c>
-      <c r="B55" s="22"/>
-      <c r="C55" s="17"/>
-      <c r="D55" s="18" t="s">
+      <c r="B55" s="19"/>
+      <c r="C55" s="14"/>
+      <c r="D55" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="E55" s="18"/>
-      <c r="F55" s="18" t="s">
+      <c r="E55" s="15"/>
+      <c r="F55" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="G55" s="19">
+      <c r="G55" s="16">
         <v>0.3</v>
       </c>
     </row>
@@ -2003,16 +1989,16 @@
       <c r="A56" s="10">
         <v>44</v>
       </c>
-      <c r="B56" s="22"/>
-      <c r="C56" s="17"/>
-      <c r="D56" s="18" t="s">
+      <c r="B56" s="19"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="E56" s="18"/>
-      <c r="F56" s="18" t="s">
+      <c r="E56" s="15"/>
+      <c r="F56" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="G56" s="19">
+      <c r="G56" s="16">
         <v>0.3</v>
       </c>
     </row>
@@ -2020,16 +2006,16 @@
       <c r="A57" s="10">
         <v>45</v>
       </c>
-      <c r="B57" s="22"/>
-      <c r="C57" s="17"/>
-      <c r="D57" s="18" t="s">
+      <c r="B57" s="19"/>
+      <c r="C57" s="14"/>
+      <c r="D57" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="E57" s="18"/>
-      <c r="F57" s="18" t="s">
+      <c r="E57" s="15"/>
+      <c r="F57" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="G57" s="19">
+      <c r="G57" s="16">
         <v>0.2</v>
       </c>
     </row>
@@ -2037,14 +2023,14 @@
       <c r="A58" s="10">
         <v>46</v>
       </c>
-      <c r="B58" s="22"/>
-      <c r="C58" s="17"/>
-      <c r="D58" s="18" t="s">
+      <c r="B58" s="19"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="E58" s="18"/>
-      <c r="F58" s="18"/>
-      <c r="G58" s="19">
+      <c r="E58" s="15"/>
+      <c r="F58" s="15"/>
+      <c r="G58" s="16">
         <v>0.2</v>
       </c>
     </row>
@@ -2052,16 +2038,16 @@
       <c r="A59" s="10">
         <v>47</v>
       </c>
-      <c r="B59" s="22"/>
-      <c r="C59" s="17"/>
-      <c r="D59" s="18" t="s">
+      <c r="B59" s="19"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="E59" s="18"/>
-      <c r="F59" s="18" t="s">
+      <c r="E59" s="15"/>
+      <c r="F59" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="G59" s="19">
+      <c r="G59" s="16">
         <v>0.2</v>
       </c>
     </row>
@@ -2069,16 +2055,16 @@
       <c r="A60" s="10">
         <v>48</v>
       </c>
-      <c r="B60" s="22"/>
-      <c r="C60" s="17"/>
-      <c r="D60" s="18" t="s">
+      <c r="B60" s="19"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="E60" s="18"/>
-      <c r="F60" s="18" t="s">
+      <c r="E60" s="15"/>
+      <c r="F60" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="G60" s="19">
+      <c r="G60" s="16">
         <v>0.2</v>
       </c>
     </row>
@@ -2086,22 +2072,22 @@
       <c r="A61" s="10">
         <v>49</v>
       </c>
-      <c r="B61" s="22" t="s">
+      <c r="B61" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C61" s="17" t="s">
+      <c r="C61" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D61" s="18" t="s">
+      <c r="D61" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E61" s="21" t="s">
+      <c r="E61" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="F61" s="18" t="s">
+      <c r="F61" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="G61" s="19">
+      <c r="G61" s="16">
         <v>0.4</v>
       </c>
       <c r="I61" s="4"/>
@@ -2110,20 +2096,20 @@
       <c r="A62" s="10">
         <v>50</v>
       </c>
-      <c r="B62" s="22"/>
-      <c r="C62" s="17" t="s">
+      <c r="B62" s="19"/>
+      <c r="C62" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D62" s="18" t="s">
+      <c r="D62" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="E62" s="21" t="s">
+      <c r="E62" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="F62" s="18" t="s">
+      <c r="F62" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="G62" s="19">
+      <c r="G62" s="16">
         <v>0.25</v>
       </c>
     </row>
@@ -2131,20 +2117,20 @@
       <c r="A63" s="10">
         <v>51</v>
       </c>
-      <c r="B63" s="22"/>
-      <c r="C63" s="17" t="s">
+      <c r="B63" s="19"/>
+      <c r="C63" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D63" s="18" t="s">
+      <c r="D63" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E63" s="21" t="s">
+      <c r="E63" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="F63" s="18" t="s">
+      <c r="F63" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G63" s="19">
+      <c r="G63" s="16">
         <v>0.3</v>
       </c>
     </row>
@@ -2152,20 +2138,20 @@
       <c r="A64" s="10">
         <v>52</v>
       </c>
-      <c r="B64" s="22"/>
-      <c r="C64" s="17" t="s">
+      <c r="B64" s="19"/>
+      <c r="C64" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D64" s="18" t="s">
+      <c r="D64" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="E64" s="21" t="s">
+      <c r="E64" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="F64" s="18" t="s">
+      <c r="F64" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G64" s="19">
+      <c r="G64" s="16">
         <v>0.3</v>
       </c>
     </row>
@@ -2173,20 +2159,20 @@
       <c r="A65" s="10">
         <v>53</v>
       </c>
-      <c r="B65" s="22" t="s">
+      <c r="B65" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C65" s="17" t="s">
+      <c r="C65" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D65" s="18" t="s">
+      <c r="D65" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="E65" s="31"/>
-      <c r="F65" s="18" t="s">
+      <c r="E65" s="17"/>
+      <c r="F65" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="G65" s="19">
+      <c r="G65" s="16">
         <v>0.1</v>
       </c>
     </row>
@@ -2194,16 +2180,16 @@
       <c r="A66" s="10">
         <v>54</v>
       </c>
-      <c r="B66" s="22"/>
-      <c r="C66" s="27" t="s">
+      <c r="B66" s="19"/>
+      <c r="C66" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D66" s="28" t="s">
+      <c r="D66" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="E66" s="32"/>
-      <c r="F66" s="33"/>
-      <c r="G66" s="29">
+      <c r="E66" s="17"/>
+      <c r="F66" s="18"/>
+      <c r="G66" s="16">
         <v>0.1</v>
       </c>
     </row>
@@ -2211,25 +2197,25 @@
       <c r="A67" s="10">
         <v>55</v>
       </c>
-      <c r="B67" s="22"/>
-      <c r="C67" s="10" t="s">
+      <c r="B67" s="19"/>
+      <c r="C67" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D67" s="13" t="s">
+      <c r="D67" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E67" s="13"/>
-      <c r="F67" s="11" t="s">
+      <c r="E67" s="17"/>
+      <c r="F67" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="G67" s="12">
+      <c r="G67" s="16">
         <v>0.3</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G68">
-        <f>SUM(G13:G67)</f>
-        <v>12.5</v>
+        <f>SUMIF(G13:G67,"RGB(0,255,0)",G13:G67)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>